<commit_message>
Mainly Trying to fix 2.7
</commit_message>
<xml_diff>
--- a/Apply introductory programming techniques/AT02/2.7 Fixed Again/Testing Log.xlsx
+++ b/Apply introductory programming techniques/AT02/2.7 Fixed Again/Testing Log.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\30007736\Desktop\Repos\Assessments\Apply introductory programming techniques\AT02\2.7 Fixed\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\30007736\Desktop\Repos\Assessments\Apply introductory programming techniques\AT02\2.7 Fixed Again\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{03054D07-3224-4611-9B38-A7C0C3717B3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{537DCA48-DEC9-4585-96A9-129694CE5AF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="6555" windowWidth="27975" windowHeight="8970" xr2:uid="{90A16CEE-6D3E-4A11-A95D-B7F4D6E71406}"/>
+    <workbookView xWindow="28935" yWindow="2445" windowWidth="15735" windowHeight="18000" xr2:uid="{90A16CEE-6D3E-4A11-A95D-B7F4D6E71406}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="12">
   <si>
     <t>Test Case</t>
   </si>
@@ -49,32 +49,35 @@
     <t>Success</t>
   </si>
   <si>
-    <t>Testing if the linear_search returns 'true' then 'false'</t>
-  </si>
-  <si>
-    <t>Should return 'true' on the first line &amp; 'false' on the second line</t>
-  </si>
-  <si>
-    <t>Returned 'false' on both lines</t>
-  </si>
-  <si>
-    <t>Returned 'true' on the first line &amp; 'false' on the second line</t>
-  </si>
-  <si>
-    <t>Testing if the linear_search returns 'true' + the index of what was searched, then 'false'</t>
-  </si>
-  <si>
-    <t>Should return 'true' + the index of what was searched on the first line &amp; 'false' on the second line</t>
-  </si>
-  <si>
-    <t>Returned 'true' + the index of what was searched on the first line &amp; 'false' on the second line</t>
+    <t>LinearSearchMethod</t>
+  </si>
+  <si>
+    <t>LinearSearchMethod 2nd Method</t>
+  </si>
+  <si>
+    <t>Testing if this works (Click this for image)</t>
+  </si>
+  <si>
+    <t>Here is the outcome (don't worry about the falses)</t>
+  </si>
+  <si>
+    <t>Testing if this works</t>
+  </si>
+  <si>
+    <t>Should print 'watermelon 1' on the first line</t>
+  </si>
+  <si>
+    <t>Should print 'watermelon 1' on the first line then print 'pineapple -1' on the second line</t>
+  </si>
+  <si>
+    <t>Here is the outcome</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,13 +92,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9B9B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9BFF9B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -107,21 +130,45 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF9B9B"/>
+      <color rgb="FF9BFF9B"/>
+      <color rgb="FFFF0000"/>
+      <color rgb="FF000000"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -430,78 +477,197 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2D44721-7C1E-400A-8A0A-BD6581E40B4F}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
+    <row r="1" spans="1:11" ht="32.25" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="2" t="s">
+    <row r="3" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="B3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="b">
-        <v>0</v>
+      <c r="C3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" s="8" t="b">
+        <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="b">
-        <v>1</v>
+    <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="5" t="b">
+        <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D5" t="b">
-        <v>1</v>
+      <c r="D5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" s="5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="H7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="5" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H3" r:id="rId1" display="Testing if the linear_search returns 'true' then 'false'" xr:uid="{D4932AA2-3858-4DA0-942F-9D045484940F}"/>
+    <hyperlink ref="J3" r:id="rId2" xr:uid="{E4720604-1F4C-4F5D-93EC-640F37053525}"/>
+    <hyperlink ref="H4" r:id="rId3" xr:uid="{881F0FC8-7904-4A09-AEFE-D5A439C47840}"/>
+    <hyperlink ref="J4" r:id="rId4" xr:uid="{E7734ED3-E6B2-4704-8C93-BAD19788CDC9}"/>
+    <hyperlink ref="H5" r:id="rId5" xr:uid="{AB236F4F-8C39-4346-865E-8D12DF4C44C4}"/>
+    <hyperlink ref="J5" r:id="rId6" xr:uid="{BDF41DCE-B6EF-4F3E-A458-461349329186}"/>
+    <hyperlink ref="B3" r:id="rId7" xr:uid="{ABF5F316-00EA-4622-A488-29CD63CA4A4D}"/>
+    <hyperlink ref="D3" r:id="rId8" xr:uid="{4B240BF1-4C1B-4E15-B043-0B1B8F213BB5}"/>
+    <hyperlink ref="B4" r:id="rId9" xr:uid="{A475351B-FE4E-4BAC-AAA3-549F9CDED59D}"/>
+    <hyperlink ref="D4" r:id="rId10" xr:uid="{FCF07688-A37C-4A58-B343-8AD17EC444D3}"/>
+    <hyperlink ref="J6:J7" r:id="rId11" display="Here is the outcome" xr:uid="{5FCBD4C1-2DC5-48EB-83A6-885973409593}"/>
+    <hyperlink ref="H6:H7" r:id="rId12" display="Testing if this works" xr:uid="{74F18ED7-D545-4E06-89C2-BD8F9F73AA41}"/>
+    <hyperlink ref="B5:B6" r:id="rId13" display="Testing if this works" xr:uid="{1D9F0E6C-772D-4C1D-8408-2B05F224C18F}"/>
+    <hyperlink ref="D5:D6" r:id="rId14" display="Here is the outcome" xr:uid="{6534B8ED-397A-4CF9-BF86-4011E57431C3}"/>
+    <hyperlink ref="H6" r:id="rId15" xr:uid="{D907E897-3D10-4110-9F88-DA8C9978A08D}"/>
+    <hyperlink ref="J6" r:id="rId16" xr:uid="{E045EC9C-531B-4E1C-9DD5-4CFE0BB8CA23}"/>
+    <hyperlink ref="B5" r:id="rId17" xr:uid="{5AA81967-4387-4820-BB3C-D4675B5F2B26}"/>
+    <hyperlink ref="D5" r:id="rId18" xr:uid="{CE0B699D-88BB-40BB-98EB-8D42D648022A}"/>
+    <hyperlink ref="H7" r:id="rId19" xr:uid="{CE3CD483-135D-44F4-931A-7F3AB34B3656}"/>
+    <hyperlink ref="J7" r:id="rId20" xr:uid="{31686D01-D3EC-48A2-AEC1-DCA81DD59F38}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed & subbitted 2.7 working on project fixing animation product diary
</commit_message>
<xml_diff>
--- a/Apply introductory programming techniques/AT02/2.7 Fixed Again/Testing Log.xlsx
+++ b/Apply introductory programming techniques/AT02/2.7 Fixed Again/Testing Log.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richa\OneDrive\Desktop\Repos\Assessments\Apply introductory programming techniques\AT02\2.7 Fixed Again\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\30007736\Desktop\Repos\Assessments\Apply introductory programming techniques\AT02\2.7 Fixed Again\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69364861-9F75-408C-B29F-D0B85A3EB031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B61887F7-5D31-4557-935B-1A6B68DEF784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{90A16CEE-6D3E-4A11-A95D-B7F4D6E71406}"/>
+    <workbookView xWindow="28680" yWindow="-6225" windowWidth="16440" windowHeight="28440" xr2:uid="{90A16CEE-6D3E-4A11-A95D-B7F4D6E71406}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="14">
   <si>
     <t>Test Case</t>
   </si>
@@ -485,30 +485,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2D44721-7C1E-400A-8A0A-BD6581E40B4F}">
   <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.88671875" customWidth="1"/>
-    <col min="3" max="3" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.44140625" customWidth="1"/>
-    <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="24" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.44140625" customWidth="1"/>
-    <col min="14" max="14" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26.77734375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.42578125" customWidth="1"/>
+    <col min="14" max="14" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="31.2" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:17" ht="32.25" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -555,7 +555,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -602,7 +602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -633,8 +633,23 @@
       <c r="K4" s="5" t="b">
         <v>0</v>
       </c>
+      <c r="M4">
+        <v>2</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q4" s="8" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -666,7 +681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -698,7 +713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -718,7 +733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="G8">
         <v>6</v>
       </c>
@@ -735,7 +750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="G9">
         <v>7</v>
       </c>
@@ -752,7 +767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="G10">
         <v>8</v>
       </c>
@@ -799,8 +814,10 @@
     <hyperlink ref="D6" r:id="rId26" xr:uid="{B67788CD-1B90-41FC-B182-951F472D3902}"/>
     <hyperlink ref="N3" r:id="rId27" xr:uid="{9C3BF73C-D063-4AEE-A1F2-B82309BC1D38}"/>
     <hyperlink ref="P3" r:id="rId28" xr:uid="{56800D98-E4A1-4042-A853-670572F35CC2}"/>
+    <hyperlink ref="N4" r:id="rId29" xr:uid="{BF5A923C-DF62-45A5-A6BB-DDB362AD498D}"/>
+    <hyperlink ref="P4" r:id="rId30" xr:uid="{5B5A20BB-CE47-4F8F-8FBA-4FACBC878FD7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId29"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId31"/>
 </worksheet>
 </file>
</xml_diff>